<commit_message>
Update published master datasets (2026-02-16)
</commit_message>
<xml_diff>
--- a/archive/InnovateUK_Funding_Opportunities_Latest_2026-02-16.xlsx
+++ b/archive/InnovateUK_Funding_Opportunities_Latest_2026-02-16.xlsx
@@ -950,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1038,21 +1038,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>European Space Agency: Sustainable Wetlands</t>
+          <t>Inclusive Mobility Challenge: Safe Urban Navigation for People with Access Needs</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/european-space-agency-sustainable-wetlands/</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/inclusive-mobility-challenge-safe-urban-navigation-for-people-with-access-needs/</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-14 10:14</t>
+          <t>2026-02-16 10:37</t>
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>46067.42638888889</v>
+        <v>46069.44236111111</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1063,21 +1063,25 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16/03/2026</t>
+          <t>16/02/2026</t>
         </is>
       </c>
       <c r="J2" s="1" t="n">
-        <v>46097</v>
+        <v>46069</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>01/05/2026                              17:00</t>
+          <t>27/03/2026                              12:00</t>
         </is>
       </c>
       <c r="L2" s="1" t="n">
-        <v>46143.70833333334</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
+        <v>46108.5</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>£500,000</t>
+        </is>
+      </c>
       <c r="N2" s="1" t="n">
         <v>46064</v>
       </c>
@@ -1085,26 +1089,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Innovate Funding Service</t>
+          <t>Innovate UK Business Connect</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
+          <t>European Space Agency: Sustainable Wetlands</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/european-space-agency-sustainable-wetlands/</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-13 10:35</t>
+          <t>2026-02-14 10:14</t>
         </is>
       </c>
       <c r="E3" s="1" t="n">
-        <v>46066.44097222222</v>
+        <v>46067.42638888889</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1113,21 +1117,23 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>16/03/2026</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>46097</v>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Wednesday 15 April 2026 11:00am</t>
+          <t>01/05/2026                              17:00</t>
         </is>
       </c>
       <c r="L3" s="1" t="n">
-        <v>46127.45833333334</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>£1.0 million</t>
-        </is>
-      </c>
+        <v>46143.70833333334</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" s="1" t="n">
         <v>46064</v>
       </c>
@@ -1135,26 +1141,26 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Innovate UK Business Connect</t>
+          <t>Innovate Funding Service</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ARIA: Scaling Trust - Tooling and Fundamental Research</t>
+          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/aria-scaling-trust-tooling-and-fundamental-research/</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-13 10:28</t>
+          <t>2026-02-13 10:35</t>
         </is>
       </c>
       <c r="E4" s="1" t="n">
-        <v>46066.43611111111</v>
+        <v>46066.44097222222</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1163,25 +1169,19 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>09/02/2026</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>46062</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>24/03/2026                              14:00</t>
+          <t>Wednesday 15 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L4" s="1" t="n">
-        <v>46105.58333333334</v>
+        <v>46127.45833333334</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>£200</t>
+          <t>£1.0 million</t>
         </is>
       </c>
       <c r="N4" s="1" t="n">
@@ -1196,12 +1196,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
+          <t>ARIA: Scaling Trust - Tooling and Fundamental Research</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/uk-germany-collaborative-innovation-for-quantum-technologies-2026/</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/aria-scaling-trust-tooling-and-fundamental-research/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1221,23 +1221,23 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>12/02/2026</t>
+          <t>09/02/2026</t>
         </is>
       </c>
       <c r="J5" s="1" t="n">
-        <v>46065</v>
+        <v>46062</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>15/04/2026                              11:00</t>
+          <t>24/03/2026                              14:00</t>
         </is>
       </c>
       <c r="L5" s="1" t="n">
-        <v>46127.45833333334</v>
+        <v>46105.58333333334</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£200</t>
         </is>
       </c>
       <c r="N5" s="1" t="n">
@@ -1252,12 +1252,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
+          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/contracts-for-innovation-in-drug-and-alcohol-addiction-healthcare/</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/uk-germany-collaborative-innovation-for-quantum-technologies-2026/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1277,23 +1277,23 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>16/02/2026</t>
+          <t>12/02/2026</t>
         </is>
       </c>
       <c r="J6" s="1" t="n">
-        <v>46069</v>
+        <v>46065</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>06/05/2026                              11:00</t>
+          <t>15/04/2026                              11:00</t>
         </is>
       </c>
       <c r="L6" s="1" t="n">
-        <v>46148.45833333334</v>
+        <v>46127.45833333334</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>£20.0 million</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N6" s="1" t="n">
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Zero Emission Flight Demonstrator Round 1</t>
+          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/zero-emission-flight-demonstrator-round-1/</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/contracts-for-innovation-in-drug-and-alcohol-addiction-healthcare/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1341,15 +1341,15 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>01/04/2026                              11:00</t>
+          <t>06/05/2026                              11:00</t>
         </is>
       </c>
       <c r="L7" s="1" t="n">
-        <v>46113.45833333334</v>
+        <v>46148.45833333334</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>£8.0 million</t>
+          <t>£20.0 million</t>
         </is>
       </c>
       <c r="N7" s="1" t="n">
@@ -1359,7 +1359,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Innovate Funding Service</t>
+          <t>Innovate UK Business Connect</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1369,16 +1369,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/zero-emission-flight-demonstrator-round-1/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-12 10:40</t>
+          <t>2026-02-13 10:28</t>
         </is>
       </c>
       <c r="E8" s="1" t="n">
-        <v>46065.44444444445</v>
+        <v>46066.43611111111</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1387,11 +1387,17 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>16/02/2026</t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>46069</v>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Wednesday 1 April 2026 11:00am</t>
+          <t>01/04/2026                              11:00</t>
         </is>
       </c>
       <c r="L8" s="1" t="n">
@@ -1399,7 +1405,7 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£8.0 million</t>
         </is>
       </c>
       <c r="N8" s="1" t="n">
@@ -1414,12 +1420,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
+          <t>Zero Emission Flight Demonstrator Round 1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1441,15 +1447,15 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Wednesday 6 May 2026 11:00am</t>
+          <t>Wednesday 1 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L9" s="1" t="n">
-        <v>46148.45833333334</v>
+        <v>46113.45833333334</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N9" s="1" t="n">
@@ -1464,12 +1470,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
+          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1499,7 +1505,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>£10.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N10" s="1" t="n">
@@ -1509,7 +1515,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Innovate UK Business Connect</t>
+          <t>Innovate Funding Service</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1519,16 +1525,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/advancing-innovation-in-drug-and-alcohol-addiction-healthcare/</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-12 10:33</t>
+          <t>2026-02-12 10:40</t>
         </is>
       </c>
       <c r="E11" s="1" t="n">
-        <v>46065.43958333333</v>
+        <v>46065.44444444445</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1537,17 +1543,11 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>16/02/2026</t>
-        </is>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>46069</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>06/05/2026                              11:00</t>
+          <t>Wednesday 6 May 2026 11:00am</t>
         </is>
       </c>
       <c r="L11" s="1" t="n">
@@ -1570,12 +1570,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Critical material recovery from e-waste recycling process by-products</t>
+          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://iuk-business-connect.org.uk/opportunities/critical-material-recovery-from-e-waste-recycling-process-by-products/</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/advancing-innovation-in-drug-and-alcohol-addiction-healthcare/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1603,14 +1603,70 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>06/05/2026                              11:00</t>
+        </is>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>46148.45833333334</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>£10.0 million</t>
+        </is>
+      </c>
+      <c r="N12" s="1" t="n">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Innovate UK Business Connect</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Critical material recovery from e-waste recycling process by-products</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://iuk-business-connect.org.uk/opportunities/critical-material-recovery-from-e-waste-recycling-process-by-products/</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2026-02-12 10:33</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>46065.43958333333</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>16/02/2026</t>
+        </is>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>46069</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>31/03/2026                              23:59</t>
         </is>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="L13" s="1" t="n">
         <v>46112.99930555555</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" s="1" t="n">
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" s="1" t="n">
         <v>46064</v>
       </c>
     </row>
@@ -1663,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -2170,7 +2226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N247"/>
+  <dimension ref="A1:N248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9413,26 +9469,26 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Innovate Funding Service</t>
+          <t>Innovate UK Business Connect</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Future Leaders Fellowships: Round 10, business and non-academic</t>
+          <t>Inclusive Mobility Challenge: Safe Urban Navigation for People with Access Needs</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2058/overview/0f904547-f415-4fb9-94a7-0701c38a2ba1</t>
+          <t>https://iuk-business-connect.org.uk/opportunities/inclusive-mobility-challenge-safe-urban-navigation-for-people-with-access-needs/</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2025-06-14 08:41</t>
+          <t>2026-02-16 10:37</t>
         </is>
       </c>
       <c r="E145" s="1" t="n">
-        <v>45822.36180555556</v>
+        <v>46069.44236111111</v>
       </c>
       <c r="F145" t="b">
         <v>1</v>
@@ -9441,23 +9497,29 @@
       <c r="H145" t="b">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr"/>
-      <c r="J145" t="inlineStr"/>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>16/02/2026</t>
+        </is>
+      </c>
+      <c r="J145" s="1" t="n">
+        <v>46069</v>
+      </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>Wednesday 5 November 2025 11:00am</t>
+          <t>27/03/2026                              12:00</t>
         </is>
       </c>
       <c r="L145" s="1" t="n">
-        <v>45966.45833333334</v>
+        <v>46108.5</v>
       </c>
       <c r="M145" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N145" s="1" t="n">
-        <v>45819</v>
+        <v>46064</v>
       </c>
     </row>
     <row r="146">
@@ -9468,12 +9530,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 2</t>
+          <t>Future Leaders Fellowships: Round 10, business and non-academic</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2223/overview/4e423e05-3228-45e3-9cfe-0b39d1227307</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2058/overview/0f904547-f415-4fb9-94a7-0701c38a2ba1</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -9495,15 +9557,15 @@
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr">
         <is>
-          <t>Thursday 24 July 2025 11:00am</t>
+          <t>Wednesday 5 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L146" s="1" t="n">
-        <v>45862.45833333334</v>
+        <v>45966.45833333334</v>
       </c>
       <c r="M146" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N146" s="1" t="n">
@@ -9518,12 +9580,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>MSI Improving energy or resource efficiency in manufacturing FS</t>
+          <t>ADOPT Facilitator Support Grant: Round 2</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2225/overview/c43ef163-3872-4178-b80d-88c406691610</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2223/overview/4e423e05-3228-45e3-9cfe-0b39d1227307</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -9545,15 +9607,15 @@
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Thursday 24 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L147" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45862.45833333334</v>
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N147" s="1" t="n">
@@ -9568,12 +9630,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>New Innovators in Marine and Maritime, Great South West</t>
+          <t>MSI Improving energy or resource efficiency in manufacturing FS</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2215/overview/67b86d6c-bab9-4a01-aacc-3da2e57edc99</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2225/overview/c43ef163-3872-4178-b80d-88c406691610</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -9603,7 +9665,7 @@
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>£50,000</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N148" s="1" t="n">
@@ -9618,12 +9680,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Autumn</t>
+          <t>New Innovators in Marine and Maritime, Great South West</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2217/overview/c555f64e-5485-4e49-89b8-32d61fac4ff0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2215/overview/67b86d6c-bab9-4a01-aacc-3da2e57edc99</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -9645,15 +9707,15 @@
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr">
         <is>
-          <t>Thursday 4 September 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L149" s="1" t="n">
-        <v>45904.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£50,000</t>
         </is>
       </c>
       <c r="N149" s="1" t="n">
@@ -9668,12 +9730,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – June 2025</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Autumn</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2218/overview/a45dcc8a-b621-4a79-9e4d-046e19b6b1e9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2217/overview/c555f64e-5485-4e49-89b8-32d61fac4ff0</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -9695,13 +9757,17 @@
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Thursday 4 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L150" s="1" t="n">
-        <v>45826.45833333334</v>
-      </c>
-      <c r="M150" t="inlineStr"/>
+        <v>45904.45833333334</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>£250,000</t>
+        </is>
+      </c>
       <c r="N150" s="1" t="n">
         <v>45819</v>
       </c>
@@ -9714,12 +9780,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Defra Farming Innovation Investor Partnership</t>
+          <t>ATI Programme strategic batch: EoI – June 2025</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2207/overview/05e5263b-75a1-49a0-87f0-261541af0840</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2218/overview/a45dcc8a-b621-4a79-9e4d-046e19b6b1e9</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -9741,17 +9807,13 @@
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L151" s="1" t="n">
-        <v>45840.45833333334</v>
-      </c>
-      <c r="M151" t="inlineStr">
-        <is>
-          <t>£3.0 million</t>
-        </is>
-      </c>
+        <v>45826.45833333334</v>
+      </c>
+      <c r="M151" t="inlineStr"/>
       <c r="N151" s="1" t="n">
         <v>45819</v>
       </c>
@@ -9764,12 +9826,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C3</t>
+          <t>Defra Farming Innovation Investor Partnership</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2204/overview/9da241b9-1fd8-49fb-b8d0-4a81a637b3b5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2207/overview/05e5263b-75a1-49a0-87f0-261541af0840</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -9791,15 +9853,15 @@
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L152" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M152" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N152" s="1" t="n">
@@ -9814,12 +9876,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 4 Discovery C3</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C3</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2200/overview/0f0721c8-5a37-4046-8e4f-7649194e8adc</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2204/overview/9da241b9-1fd8-49fb-b8d0-4a81a637b3b5</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -9864,12 +9926,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Scaling community initiatives in diet and exercise</t>
+          <t>Ofgem Strategic Innovation Fund Round 4 Discovery C3</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2191/overview/6a097cf8-8f81-495d-b56f-3f240cfde64c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2200/overview/0f0721c8-5a37-4046-8e4f-7649194e8adc</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -9891,15 +9953,15 @@
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L154" s="1" t="n">
-        <v>45826.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N154" s="1" t="n">
@@ -9914,12 +9976,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Quantum Sensors and PNT Missions Primer</t>
+          <t>Contracts for Innovation: Scaling community initiatives in diet and exercise</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2209/overview/28f8801b-a8b3-48c8-8c81-64d75341b81d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2191/overview/6a097cf8-8f81-495d-b56f-3f240cfde64c</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -9941,15 +10003,15 @@
       <c r="J155" t="inlineStr"/>
       <c r="K155" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L155" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45826.45833333334</v>
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N155" s="1" t="n">
@@ -9964,12 +10026,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Net Zero Living Tech Trials, phase 3</t>
+          <t>Contracts for Innovation: Quantum Sensors and PNT Missions Primer</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2189/overview/a59ac38e-662b-49a5-b7f9-a44c2cc38c61</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2209/overview/28f8801b-a8b3-48c8-8c81-64d75341b81d</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -9991,15 +10053,15 @@
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L156" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N156" s="1" t="n">
@@ -10014,12 +10076,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Clean Air, Phase 3</t>
+          <t>Contracts for Innovation: Net Zero Living Tech Trials, phase 3</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2181/overview/02aad9d2-c984-4bd5-a3f6-80f25ec62870</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2189/overview/a59ac38e-662b-49a5-b7f9-a44c2cc38c61</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -10064,12 +10126,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: DSbD Advancing CHERI Tools and software</t>
+          <t>Contracts for Innovation: Clean Air, Phase 3</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2194/overview/91c68630-20eb-4247-8296-ae1737637756</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2181/overview/02aad9d2-c984-4bd5-a3f6-80f25ec62870</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -10091,15 +10153,15 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr">
         <is>
-          <t>Wednesday 18 June 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L158" s="1" t="n">
-        <v>45826.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M158" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N158" s="1" t="n">
@@ -10114,12 +10176,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: DSbD Advancing CHERI RISC-V Devices</t>
+          <t>Contracts for Innovation: DSbD Advancing CHERI Tools and software</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2198/overview/b2e2fd41-d372-4e33-a6df-8bfefb8de0f9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2194/overview/91c68630-20eb-4247-8296-ae1737637756</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -10149,7 +10211,7 @@
       </c>
       <c r="M159" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N159" s="1" t="n">
@@ -10164,12 +10226,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Canada-UK Semiconductors</t>
+          <t>Contracts for Innovation: DSbD Advancing CHERI RISC-V Devices</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2192/overview/3906cbd5-fec2-4c1f-897d-ccab071708b3</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2198/overview/b2e2fd41-d372-4e33-a6df-8bfefb8de0f9</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -10191,15 +10253,15 @@
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 18 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L160" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45826.45833333334</v>
       </c>
       <c r="M160" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N160" s="1" t="n">
@@ -10214,12 +10276,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Accelerated Knowledge Transfer 4 (AKT4) Addiction</t>
+          <t>Canada-UK Semiconductors</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2178/overview/2699060f-dd6f-415b-ae47-bead15aa430e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2192/overview/3906cbd5-fec2-4c1f-897d-ccab071708b3</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -10241,15 +10303,15 @@
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L161" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45945.45833333334</v>
       </c>
       <c r="M161" t="inlineStr">
         <is>
-          <t>£35,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N161" s="1" t="n">
@@ -10264,12 +10326,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Innovate UK innovation loans future economy: Round 21</t>
+          <t>Accelerated Knowledge Transfer 4 (AKT4) Addiction</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2188/overview/20c89a26-2479-4f80-b35a-b62ed3b9b3ce</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2178/overview/2699060f-dd6f-415b-ae47-bead15aa430e</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -10299,7 +10361,7 @@
       </c>
       <c r="M162" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£35,000</t>
         </is>
       </c>
       <c r="N162" s="1" t="n">
@@ -10314,12 +10376,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Farming Futures R&amp;D Fund: Precision Breeding Competition</t>
+          <t>Innovate UK innovation loans future economy: Round 21</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2168/overview/0fef9171-75b0-4f3e-acef-42920e7e5d5e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2188/overview/20c89a26-2479-4f80-b35a-b62ed3b9b3ce</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -10341,15 +10403,15 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L163" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M163" t="inlineStr">
         <is>
-          <t>£2.5 million</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N163" s="1" t="n">
@@ -10364,12 +10426,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Farming Futures R&amp;D Fund: low emissions farming</t>
+          <t>Farming Futures R&amp;D Fund: Precision Breeding Competition</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2169/overview/64b0d550-3f46-4ab4-a0cd-5fa7ac488cb6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2168/overview/0fef9171-75b0-4f3e-acef-42920e7e5d5e</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -10414,12 +10476,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Investor Partnerships: Clean Energy and Climate Technologies</t>
+          <t>Farming Futures R&amp;D Fund: low emissions farming</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2175/overview/7487b4f1-51e6-4f15-a4c8-f103559d14bb</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2169/overview/64b0d550-3f46-4ab4-a0cd-5fa7ac488cb6</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -10441,15 +10503,15 @@
       <c r="J165" t="inlineStr"/>
       <c r="K165" t="inlineStr">
         <is>
-          <t>Wednesday 2 July 2025 11:00am</t>
+          <t>Wednesday 25 June 2025 11:00am</t>
         </is>
       </c>
       <c r="L165" s="1" t="n">
-        <v>45840.45833333334</v>
+        <v>45833.45833333334</v>
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£2.5 million</t>
         </is>
       </c>
       <c r="N165" s="1" t="n">
@@ -10464,12 +10526,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 1</t>
+          <t>Investor Partnerships: Clean Energy and Climate Technologies</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2162/overview/c35de0a9-5072-4142-8a52-1cdce8ef3871</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2175/overview/7487b4f1-51e6-4f15-a4c8-f103559d14bb</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -10491,15 +10553,15 @@
       <c r="J166" t="inlineStr"/>
       <c r="K166" t="inlineStr">
         <is>
-          <t>Wednesday 25 June 2025 11:00am</t>
+          <t>Wednesday 2 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L166" s="1" t="n">
-        <v>45833.45833333334</v>
+        <v>45840.45833333334</v>
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N166" s="1" t="n">
@@ -10514,12 +10576,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Horizon Europe Guarantee - EIT KICs 2023</t>
+          <t>Full ADOPT Grant: Round 1</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1585/overview/32135a71-171a-46bf-ad56-e2e65a1a3574</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2162/overview/c35de0a9-5072-4142-8a52-1cdce8ef3871</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -10541,11 +10603,17 @@
       <c r="J167" t="inlineStr"/>
       <c r="K167" t="inlineStr">
         <is>
-          <t>Thursday 27 November 2025 4:00pm</t>
-        </is>
-      </c>
-      <c r="L167" t="inlineStr"/>
-      <c r="M167" t="inlineStr"/>
+          <t>Wednesday 25 June 2025 11:00am</t>
+        </is>
+      </c>
+      <c r="L167" s="1" t="n">
+        <v>45833.45833333334</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>£100,000</t>
+        </is>
+      </c>
       <c r="N167" s="1" t="n">
         <v>45819</v>
       </c>
@@ -10558,12 +10626,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Horizon Europe Guarantee Extension</t>
+          <t>Horizon Europe Guarantee - EIT KICs 2023</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1389/overview/b900fdc4-c48d-4d8a-8733-ce4ca210ae9a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1585/overview/32135a71-171a-46bf-ad56-e2e65a1a3574</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -10602,21 +10670,21 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 3</t>
+          <t>Horizon Europe Guarantee Extension</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2184/overview/c599b17c-e13a-4e13-995e-53cc4d4508a1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/1389/overview/b900fdc4-c48d-4d8a-8733-ce4ca210ae9a</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>2025-06-16 22:04</t>
+          <t>2025-06-14 08:41</t>
         </is>
       </c>
       <c r="E169" s="1" t="n">
-        <v>45824.91944444444</v>
+        <v>45822.36180555556</v>
       </c>
       <c r="F169" t="b">
         <v>1</v>
@@ -10629,17 +10697,11 @@
       <c r="J169" t="inlineStr"/>
       <c r="K169" t="inlineStr">
         <is>
-          <t>Wednesday 17 September 2025 11:00am</t>
-        </is>
-      </c>
-      <c r="L169" s="1" t="n">
-        <v>45917.45833333334</v>
-      </c>
-      <c r="M169" t="inlineStr">
-        <is>
-          <t>£8,500</t>
-        </is>
-      </c>
+          <t>Thursday 27 November 2025 4:00pm</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
       <c r="N169" s="1" t="n">
         <v>45819</v>
       </c>
@@ -10652,21 +10714,21 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Agri-tech and food technology, Mid and North Wales - CRD</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 3</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2212/overview/4411087f-2a92-4aed-b735-d1a813376bec</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2184/overview/c599b17c-e13a-4e13-995e-53cc4d4508a1</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>2025-06-26 08:52</t>
+          <t>2025-06-16 22:04</t>
         </is>
       </c>
       <c r="E170" s="1" t="n">
-        <v>45834.36944444444</v>
+        <v>45824.91944444444</v>
       </c>
       <c r="F170" t="b">
         <v>1</v>
@@ -10679,19 +10741,19 @@
       <c r="J170" t="inlineStr"/>
       <c r="K170" t="inlineStr">
         <is>
-          <t>Wednesday 20 August 2025 11:00am</t>
+          <t>Wednesday 17 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L170" s="1" t="n">
-        <v>45889.45833333334</v>
+        <v>45917.45833333334</v>
       </c>
       <c r="M170" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N170" s="1" t="n">
-        <v>45833</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="171">
@@ -10702,12 +10764,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 2</t>
+          <t>Agri-tech and food technology, Mid and North Wales - CRD</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2222/overview/c3d5b2f9-e4d4-4ddc-99a2-589904ac3d42</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2212/overview/4411087f-2a92-4aed-b735-d1a813376bec</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -10737,7 +10799,7 @@
       </c>
       <c r="M171" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N171" s="1" t="n">
@@ -10752,21 +10814,21 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 22</t>
+          <t>Full ADOPT Grant Round 2</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2236/overview/70cbae59-4e67-4626-8cb0-6bbbfc0cf6b7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2222/overview/c3d5b2f9-e4d4-4ddc-99a2-589904ac3d42</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2025-07-03 08:52</t>
+          <t>2025-06-26 08:52</t>
         </is>
       </c>
       <c r="E172" s="1" t="n">
-        <v>45841.36944444444</v>
+        <v>45834.36944444444</v>
       </c>
       <c r="F172" t="b">
         <v>1</v>
@@ -10779,19 +10841,19 @@
       <c r="J172" t="inlineStr"/>
       <c r="K172" t="inlineStr">
         <is>
-          <t>Wednesday 27 August 2025 11:00am</t>
+          <t>Wednesday 20 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L172" s="1" t="n">
-        <v>45896.45833333334</v>
+        <v>45889.45833333334</v>
       </c>
       <c r="M172" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N172" s="1" t="n">
-        <v>45840</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="173">
@@ -10802,21 +10864,21 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Growth Catalyst Early Stage: New Innovators</t>
+          <t>Innovate UK Innovation Loans Round 22</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2220/overview/bcfd2780-f307-4434-be32-46889a239024</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2236/overview/70cbae59-4e67-4626-8cb0-6bbbfc0cf6b7</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>2025-07-07 08:54</t>
+          <t>2025-07-03 08:52</t>
         </is>
       </c>
       <c r="E173" s="1" t="n">
-        <v>45845.37083333333</v>
+        <v>45841.36944444444</v>
       </c>
       <c r="F173" t="b">
         <v>1</v>
@@ -10829,15 +10891,15 @@
       <c r="J173" t="inlineStr"/>
       <c r="K173" t="inlineStr">
         <is>
-          <t>Wednesday 6 August 2025 11:00am</t>
+          <t>Wednesday 27 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L173" s="1" t="n">
-        <v>45875.45833333334</v>
+        <v>45896.45833333334</v>
       </c>
       <c r="M173" t="inlineStr">
         <is>
-          <t>£50,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N173" s="1" t="n">
@@ -10852,12 +10914,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – July 2025</t>
+          <t>Growth Catalyst Early Stage: New Innovators</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2228/overview/5ccf059d-ae66-4f72-a319-4b12cbd46d1c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2220/overview/bcfd2780-f307-4434-be32-46889a239024</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -10879,13 +10941,17 @@
       <c r="J174" t="inlineStr"/>
       <c r="K174" t="inlineStr">
         <is>
-          <t>Wednesday 23 July 2025 11:00am</t>
+          <t>Wednesday 6 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L174" s="1" t="n">
-        <v>45861.45833333334</v>
-      </c>
-      <c r="M174" t="inlineStr"/>
+        <v>45875.45833333334</v>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>£50,000</t>
+        </is>
+      </c>
       <c r="N174" s="1" t="n">
         <v>45840</v>
       </c>
@@ -10898,21 +10964,21 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Construction Impacts</t>
+          <t>ATI Programme strategic batch: EoI – July 2025</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2242/overview/51b1338a-0d60-43de-b062-fe7a48a7d42f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2228/overview/5ccf059d-ae66-4f72-a319-4b12cbd46d1c</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>2025-07-09 08:54</t>
+          <t>2025-07-07 08:54</t>
         </is>
       </c>
       <c r="E175" s="1" t="n">
-        <v>45847.37083333333</v>
+        <v>45845.37083333333</v>
       </c>
       <c r="F175" t="b">
         <v>1</v>
@@ -10925,19 +10991,15 @@
       <c r="J175" t="inlineStr"/>
       <c r="K175" t="inlineStr">
         <is>
-          <t>Wednesday 27 August 2025 11:00am</t>
+          <t>Wednesday 23 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L175" s="1" t="n">
-        <v>45896.45833333334</v>
-      </c>
-      <c r="M175" t="inlineStr">
-        <is>
-          <t>£300,000</t>
-        </is>
-      </c>
+        <v>45861.45833333334</v>
+      </c>
+      <c r="M175" t="inlineStr"/>
       <c r="N175" s="1" t="n">
-        <v>45847</v>
+        <v>45840</v>
       </c>
     </row>
     <row r="176">
@@ -10948,12 +11010,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Chemicals Impacts</t>
+          <t>Contracts for Innovation: Resource Efficient Construction Impacts</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2240/overview/10f28eca-01f0-4abf-8e0c-998151fe747b</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2242/overview/51b1338a-0d60-43de-b062-fe7a48a7d42f</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -10998,12 +11060,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Resource Efficient Automotive Impacts</t>
+          <t>Contracts for Innovation: Resource Efficient Chemicals Impacts</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2241/overview/baec7aff-ca8b-456c-9e4d-d6eb9621a988</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2240/overview/10f28eca-01f0-4abf-8e0c-998151fe747b</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -11048,12 +11110,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Future Flight: Regional Demonstrator 2</t>
+          <t>Contracts for Innovation: Resource Efficient Automotive Impacts</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2239/overview/7c5a9acd-4b31-414a-8e35-20dd1df3a2a1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2241/overview/baec7aff-ca8b-456c-9e4d-d6eb9621a988</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -11075,15 +11137,15 @@
       <c r="J178" t="inlineStr"/>
       <c r="K178" t="inlineStr">
         <is>
-          <t>Thursday 17 July 2025 11:00am</t>
+          <t>Wednesday 27 August 2025 11:00am</t>
         </is>
       </c>
       <c r="L178" s="1" t="n">
-        <v>45855.45833333334</v>
+        <v>45896.45833333334</v>
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>£200,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N178" s="1" t="n">
@@ -11098,21 +11160,21 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up: Feasibility Studies</t>
+          <t>Future Flight: Regional Demonstrator 2</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2247/overview/53da287a-c141-48d2-a3eb-f854e14c6578</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2239/overview/7c5a9acd-4b31-414a-8e35-20dd1df3a2a1</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>2025-07-15 08:20</t>
+          <t>2025-07-09 08:54</t>
         </is>
       </c>
       <c r="E179" s="1" t="n">
-        <v>45853.34722222222</v>
+        <v>45847.37083333333</v>
       </c>
       <c r="F179" t="b">
         <v>1</v>
@@ -11125,15 +11187,15 @@
       <c r="J179" t="inlineStr"/>
       <c r="K179" t="inlineStr">
         <is>
-          <t>Wednesday 3 September 2025 11:00am</t>
+          <t>Thursday 17 July 2025 11:00am</t>
         </is>
       </c>
       <c r="L179" s="1" t="n">
-        <v>45903.45833333334</v>
+        <v>45855.45833333334</v>
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>£750,000</t>
+          <t>£200,000</t>
         </is>
       </c>
       <c r="N179" s="1" t="n">
@@ -11148,12 +11210,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Demonstrate</t>
+          <t>DRIVE35 Scale-up: Feasibility Studies</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2245/overview/777781a3-f181-42b3-a05e-86b96754f28d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2247/overview/53da287a-c141-48d2-a3eb-f854e14c6578</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -11175,15 +11237,15 @@
       <c r="J180" t="inlineStr"/>
       <c r="K180" t="inlineStr">
         <is>
-          <t>Wednesday 1 October 2025 11:00am</t>
+          <t>Wednesday 3 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L180" s="1" t="n">
-        <v>45931.45833333334</v>
+        <v>45903.45833333334</v>
       </c>
       <c r="M180" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£750,000</t>
         </is>
       </c>
       <c r="N180" s="1" t="n">
@@ -11198,12 +11260,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Collaborate</t>
+          <t>DRIVE35 Innovation Fund: Demonstrate</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2244/overview/84f81488-4936-4551-a315-7ec40cf1065d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2245/overview/777781a3-f181-42b3-a05e-86b96754f28d</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -11233,7 +11295,7 @@
       </c>
       <c r="M181" t="inlineStr">
         <is>
-          <t>£25.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N181" s="1" t="n">
@@ -11248,21 +11310,21 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 3</t>
+          <t>DRIVE35 Innovation Fund: Collaborate</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2251/overview/f40e861a-c7f6-4597-ac5d-2e8d1b4f59f8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2244/overview/84f81488-4936-4551-a315-7ec40cf1065d</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>2025-07-25 08:20</t>
+          <t>2025-07-15 08:20</t>
         </is>
       </c>
       <c r="E182" s="1" t="n">
-        <v>45863.34722222222</v>
+        <v>45853.34722222222</v>
       </c>
       <c r="F182" t="b">
         <v>1</v>
@@ -11275,19 +11337,19 @@
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr">
         <is>
-          <t>Wednesday 3 September 2025 11:00am</t>
+          <t>Wednesday 1 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L182" s="1" t="n">
-        <v>45903.45833333334</v>
+        <v>45931.45833333334</v>
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£25.0 million</t>
         </is>
       </c>
       <c r="N182" s="1" t="n">
-        <v>45861</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="183">
@@ -11298,21 +11360,21 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Sovereign AI - Proof of concept</t>
+          <t>ADOPT Facilitator Support Grant: Round 3</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2259/overview/9061ddb2-fa12-45c9-8691-d36649c96e9c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2251/overview/f40e861a-c7f6-4597-ac5d-2e8d1b4f59f8</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>2025-08-07 08:21</t>
+          <t>2025-07-25 08:20</t>
         </is>
       </c>
       <c r="E183" s="1" t="n">
-        <v>45876.34791666667</v>
+        <v>45863.34722222222</v>
       </c>
       <c r="F183" t="b">
         <v>1</v>
@@ -11325,19 +11387,19 @@
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr">
         <is>
-          <t>Wednesday 10 September 2025 11:00am</t>
+          <t>Wednesday 3 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L183" s="1" t="n">
-        <v>45910.45833333334</v>
+        <v>45903.45833333334</v>
       </c>
       <c r="M183" t="inlineStr">
         <is>
-          <t>£120,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N183" s="1" t="n">
-        <v>45875</v>
+        <v>45861</v>
       </c>
     </row>
     <row r="184">
@@ -11348,21 +11410,21 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 3</t>
+          <t>Sovereign AI - Proof of concept</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2186/overview/e51c18bc-21b3-450d-bdbc-2f43dad3b268</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2259/overview/9061ddb2-fa12-45c9-8691-d36649c96e9c</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>2025-08-14 08:20</t>
+          <t>2025-08-07 08:21</t>
         </is>
       </c>
       <c r="E184" s="1" t="n">
-        <v>45883.34722222222</v>
+        <v>45876.34791666667</v>
       </c>
       <c r="F184" t="b">
         <v>1</v>
@@ -11375,19 +11437,19 @@
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 10 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L184" s="1" t="n">
-        <v>45980.45833333334</v>
+        <v>45910.45833333334</v>
       </c>
       <c r="M184" t="inlineStr">
         <is>
-          <t>£8.0 million</t>
+          <t>£120,000</t>
         </is>
       </c>
       <c r="N184" s="1" t="n">
-        <v>45882</v>
+        <v>45875</v>
       </c>
     </row>
     <row r="185">
@@ -11398,12 +11460,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 2</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 3</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2185/overview/d5b2aeb3-c2e4-4d78-9be3-f1d9919b0956</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2186/overview/e51c18bc-21b3-450d-bdbc-2f43dad3b268</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -11433,7 +11495,7 @@
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>£4.5 million</t>
+          <t>£8.0 million</t>
         </is>
       </c>
       <c r="N185" s="1" t="n">
@@ -11448,12 +11510,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Obesity Pathway Innovation Programme (OPIP): Strand 1</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 2</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2177/overview/696c1e3c-589d-4c37-8958-6255d1dc125a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2185/overview/d5b2aeb3-c2e4-4d78-9be3-f1d9919b0956</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -11483,7 +11545,7 @@
       </c>
       <c r="M186" t="inlineStr">
         <is>
-          <t>£3.5 million</t>
+          <t>£4.5 million</t>
         </is>
       </c>
       <c r="N186" s="1" t="n">
@@ -11498,21 +11560,21 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Analysis for Innovators: National Physical Laboratory Stage 1</t>
+          <t>Obesity Pathway Innovation Programme (OPIP): Strand 1</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2266/overview/2fcad3ee-b5d6-4f01-8b1a-0e1af3c93023</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2177/overview/696c1e3c-589d-4c37-8958-6255d1dc125a</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>2025-08-26 08:20</t>
+          <t>2025-08-14 08:20</t>
         </is>
       </c>
       <c r="E187" s="1" t="n">
-        <v>45895.34722222222</v>
+        <v>45883.34722222222</v>
       </c>
       <c r="F187" t="b">
         <v>1</v>
@@ -11525,19 +11587,19 @@
       <c r="J187" t="inlineStr"/>
       <c r="K187" t="inlineStr">
         <is>
-          <t>Wednesday 10 September 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L187" s="1" t="n">
-        <v>45910.45833333334</v>
+        <v>45980.45833333334</v>
       </c>
       <c r="M187" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£3.5 million</t>
         </is>
       </c>
       <c r="N187" s="1" t="n">
-        <v>45889</v>
+        <v>45882</v>
       </c>
     </row>
     <row r="188">
@@ -11548,21 +11610,21 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 3</t>
+          <t>Analysis for Innovators: National Physical Laboratory Stage 1</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2265/overview/fae182db-d9e5-4173-bb59-8fde361ccad4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2266/overview/2fcad3ee-b5d6-4f01-8b1a-0e1af3c93023</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>2025-08-27 08:18</t>
+          <t>2025-08-26 08:20</t>
         </is>
       </c>
       <c r="E188" s="1" t="n">
-        <v>45896.34583333333</v>
+        <v>45895.34722222222</v>
       </c>
       <c r="F188" t="b">
         <v>1</v>
@@ -11575,11 +11637,11 @@
       <c r="J188" t="inlineStr"/>
       <c r="K188" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 10 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L188" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45910.45833333334</v>
       </c>
       <c r="M188" t="inlineStr">
         <is>
@@ -11587,7 +11649,7 @@
         </is>
       </c>
       <c r="N188" s="1" t="n">
-        <v>45896</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="189">
@@ -11598,21 +11660,21 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch: EoI – September 2025</t>
+          <t>Full ADOPT Grant Round 3</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2273/overview/b30df196-a9a2-4e53-85e1-e3e6aaa5c5b7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2265/overview/fae182db-d9e5-4173-bb59-8fde361ccad4</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>2025-09-01 08:20</t>
+          <t>2025-08-27 08:18</t>
         </is>
       </c>
       <c r="E189" s="1" t="n">
-        <v>45901.34722222222</v>
+        <v>45896.34583333333</v>
       </c>
       <c r="F189" t="b">
         <v>1</v>
@@ -11625,13 +11687,17 @@
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr">
         <is>
-          <t>Wednesday 17 September 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L189" s="1" t="n">
-        <v>45917.45833333334</v>
-      </c>
-      <c r="M189" t="inlineStr"/>
+        <v>45945.45833333334</v>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>£100,000</t>
+        </is>
+      </c>
       <c r="N189" s="1" t="n">
         <v>45896</v>
       </c>
@@ -11644,21 +11710,21 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Farming Innovation Programme: Small R&amp;D Partnership Projects Rd 4</t>
+          <t>ATI Programme strategic batch: EoI – September 2025</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2010/overview/bcd5cf06-313c-4197-ae47-0035f674717f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2273/overview/b30df196-a9a2-4e53-85e1-e3e6aaa5c5b7</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2025-09-02 08:19</t>
+          <t>2025-09-01 08:20</t>
         </is>
       </c>
       <c r="E190" s="1" t="n">
-        <v>45902.34652777778</v>
+        <v>45901.34722222222</v>
       </c>
       <c r="F190" t="b">
         <v>1</v>
@@ -11671,17 +11737,13 @@
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr">
         <is>
-          <t>Wednesday 5 November 2025 11:00am</t>
+          <t>Wednesday 17 September 2025 11:00am</t>
         </is>
       </c>
       <c r="L190" s="1" t="n">
-        <v>45966.45833333334</v>
-      </c>
-      <c r="M190" t="inlineStr">
-        <is>
-          <t>£3.0 million</t>
-        </is>
-      </c>
+        <v>45917.45833333334</v>
+      </c>
+      <c r="M190" t="inlineStr"/>
       <c r="N190" s="1" t="n">
         <v>45896</v>
       </c>
@@ -11694,21 +11756,21 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 4</t>
+          <t>Farming Innovation Programme: Small R&amp;D Partnership Projects Rd 4</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2277/overview/7386173a-c074-4617-b7d0-f54f3a458247</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2010/overview/bcd5cf06-313c-4197-ae47-0035f674717f</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2025-09-04 08:18</t>
+          <t>2025-09-02 08:19</t>
         </is>
       </c>
       <c r="E191" s="1" t="n">
-        <v>45904.34583333333</v>
+        <v>45902.34652777778</v>
       </c>
       <c r="F191" t="b">
         <v>1</v>
@@ -11721,19 +11783,19 @@
       <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Wednesday 5 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L191" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45966.45833333334</v>
       </c>
       <c r="M191" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N191" s="1" t="n">
-        <v>45903</v>
+        <v>45896</v>
       </c>
     </row>
     <row r="192">
@@ -11744,21 +11806,21 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 23</t>
+          <t>ADOPT Facilitator Support Grant: Round 4</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2275/overview/dec9b656-5f30-414e-a169-e11e17d04896</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2277/overview/7386173a-c074-4617-b7d0-f54f3a458247</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>2025-09-05 08:18</t>
+          <t>2025-09-04 08:18</t>
         </is>
       </c>
       <c r="E192" s="1" t="n">
-        <v>45905.34583333333</v>
+        <v>45904.34583333333</v>
       </c>
       <c r="F192" t="b">
         <v>1</v>
@@ -11771,15 +11833,15 @@
       <c r="J192" t="inlineStr"/>
       <c r="K192" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Wednesday 15 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L192" s="1" t="n">
-        <v>45952.45833333334</v>
+        <v>45945.45833333334</v>
       </c>
       <c r="M192" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N192" s="1" t="n">
@@ -11794,21 +11856,21 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>UK-Netherlands Co-Innovation and Testbeds Pilot for Quantum Tech</t>
+          <t>Innovate UK Innovation Loans Round 23</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2288/overview/d547d84e-d652-4ed6-9c85-b12ab8d785d2</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2275/overview/dec9b656-5f30-414e-a169-e11e17d04896</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>2025-09-12 08:17</t>
+          <t>2025-09-05 08:18</t>
         </is>
       </c>
       <c r="E193" s="1" t="n">
-        <v>45912.34513888889</v>
+        <v>45905.34583333333</v>
       </c>
       <c r="F193" t="b">
         <v>1</v>
@@ -11821,19 +11883,19 @@
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr">
         <is>
-          <t>Tuesday 28 October 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L193" s="1" t="n">
-        <v>45958.45833333334</v>
+        <v>45952.45833333334</v>
       </c>
       <c r="M193" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N193" s="1" t="n">
-        <v>45910</v>
+        <v>45903</v>
       </c>
     </row>
     <row r="194">
@@ -11844,21 +11906,21 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Contracts for Innovation: Quantum Technologies for Transport - Phase 1</t>
+          <t>UK-Netherlands Co-Innovation and Testbeds Pilot for Quantum Tech</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2292/overview/cdea3182-7495-4cad-8435-f49882f08ec7</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2288/overview/d547d84e-d652-4ed6-9c85-b12ab8d785d2</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>2025-09-16 08:19</t>
+          <t>2025-09-12 08:17</t>
         </is>
       </c>
       <c r="E194" s="1" t="n">
-        <v>45916.34652777778</v>
+        <v>45912.34513888889</v>
       </c>
       <c r="F194" t="b">
         <v>1</v>
@@ -11871,15 +11933,15 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr">
         <is>
-          <t>Wednesday 15 October 2025 11:00am</t>
+          <t>Tuesday 28 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L194" s="1" t="n">
-        <v>45945.45833333334</v>
+        <v>45958.45833333334</v>
       </c>
       <c r="M194" t="inlineStr">
         <is>
-          <t>£40,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N194" s="1" t="n">
@@ -11894,21 +11956,21 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up Fund</t>
+          <t>Contracts for Innovation: Quantum Technologies for Transport - Phase 1</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2279/overview/029bd996-9abd-42d9-8134-e2d34e3cfff5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2292/overview/cdea3182-7495-4cad-8435-f49882f08ec7</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>2025-09-17 08:18</t>
+          <t>2025-09-16 08:19</t>
         </is>
       </c>
       <c r="E195" s="1" t="n">
-        <v>45917.34583333333</v>
+        <v>45916.34652777778</v>
       </c>
       <c r="F195" t="b">
         <v>1</v>
@@ -11921,17 +11983,19 @@
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr">
         <is>
-          <t>There is no submission deadline</t>
-        </is>
-      </c>
-      <c r="L195" t="inlineStr"/>
+          <t>Wednesday 15 October 2025 11:00am</t>
+        </is>
+      </c>
+      <c r="L195" s="1" t="n">
+        <v>45945.45833333334</v>
+      </c>
       <c r="M195" t="inlineStr">
         <is>
-          <t>£20.0 million</t>
+          <t>£40,000</t>
         </is>
       </c>
       <c r="N195" s="1" t="n">
-        <v>45917</v>
+        <v>45910</v>
       </c>
     </row>
     <row r="196">
@@ -11942,21 +12006,21 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Winter</t>
+          <t>DRIVE35 Scale-up Fund</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2295/overview/cdce9dab-263c-444b-9e91-61f13046bd62</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2279/overview/029bd996-9abd-42d9-8134-e2d34e3cfff5</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>2025-09-18 08:17</t>
+          <t>2025-09-17 08:18</t>
         </is>
       </c>
       <c r="E196" s="1" t="n">
-        <v>45918.34513888889</v>
+        <v>45917.34583333333</v>
       </c>
       <c r="F196" t="b">
         <v>1</v>
@@ -11969,15 +12033,13 @@
       <c r="J196" t="inlineStr"/>
       <c r="K196" t="inlineStr">
         <is>
-          <t>Thursday 4 December 2025 11:00am</t>
-        </is>
-      </c>
-      <c r="L196" s="1" t="n">
-        <v>45995.45833333334</v>
-      </c>
+          <t>There is no submission deadline</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr"/>
       <c r="M196" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£20.0 million</t>
         </is>
       </c>
       <c r="N196" s="1" t="n">
@@ -11992,21 +12054,21 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Resource efficiency for resilience and sustainability FS</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Winter</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2293/overview/2efee934-8622-4686-bc02-a6ac7fc9e5a6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2295/overview/cdce9dab-263c-444b-9e91-61f13046bd62</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>2025-09-20 08:16</t>
+          <t>2025-09-18 08:17</t>
         </is>
       </c>
       <c r="E197" s="1" t="n">
-        <v>45920.34444444445</v>
+        <v>45918.34513888889</v>
       </c>
       <c r="F197" t="b">
         <v>1</v>
@@ -12019,15 +12081,15 @@
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr">
         <is>
-          <t>Monday 3 November 2025 11:00am</t>
+          <t>Thursday 4 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L197" s="1" t="n">
-        <v>45964.45833333334</v>
+        <v>45995.45833333334</v>
       </c>
       <c r="M197" t="inlineStr">
         <is>
-          <t>£25,000</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N197" s="1" t="n">
@@ -12042,21 +12104,21 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C4</t>
+          <t>Resource efficiency for resilience and sustainability FS</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2284/overview/aa6bd2b1-f6e1-4e96-bd4c-0557c10779c8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2293/overview/2efee934-8622-4686-bc02-a6ac7fc9e5a6</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>2025-09-23 08:18</t>
+          <t>2025-09-20 08:16</t>
         </is>
       </c>
       <c r="E198" s="1" t="n">
-        <v>45923.34583333333</v>
+        <v>45920.34444444445</v>
       </c>
       <c r="F198" t="b">
         <v>1</v>
@@ -12069,15 +12131,15 @@
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Monday 3 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L198" s="1" t="n">
-        <v>45952.45833333334</v>
+        <v>45964.45833333334</v>
       </c>
       <c r="M198" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£25,000</t>
         </is>
       </c>
       <c r="N198" s="1" t="n">
@@ -12092,21 +12154,21 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Farming Innovation Programme: Feasibility Round 4</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C4</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2006/overview/b67973b5-6d46-4a34-a864-bec1212e3fe0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2284/overview/aa6bd2b1-f6e1-4e96-bd4c-0557c10779c8</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>2025-09-29 08:20</t>
+          <t>2025-09-23 08:18</t>
         </is>
       </c>
       <c r="E199" s="1" t="n">
-        <v>45929.34722222222</v>
+        <v>45923.34583333333</v>
       </c>
       <c r="F199" t="b">
         <v>1</v>
@@ -12119,19 +12181,19 @@
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr">
         <is>
-          <t>Wednesday 3 December 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L199" s="1" t="n">
-        <v>45994.45833333334</v>
+        <v>45952.45833333334</v>
       </c>
       <c r="M199" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N199" s="1" t="n">
-        <v>45924</v>
+        <v>45917</v>
       </c>
     </row>
     <row r="200">
@@ -12142,21 +12204,21 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Eureka GlobalStars Japan 2026</t>
+          <t>Farming Innovation Programme: Feasibility Round 4</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2276/overview/19635c62-dd91-41d8-a90e-547cdb5acbfa</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2006/overview/b67973b5-6d46-4a34-a864-bec1212e3fe0</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>2025-10-03 08:17</t>
+          <t>2025-09-29 08:20</t>
         </is>
       </c>
       <c r="E200" s="1" t="n">
-        <v>45933.34513888889</v>
+        <v>45929.34722222222</v>
       </c>
       <c r="F200" t="b">
         <v>1</v>
@@ -12169,19 +12231,19 @@
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="inlineStr">
         <is>
-          <t>Wednesday 21 January 2026 11:00am</t>
+          <t>Wednesday 3 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L200" s="1" t="n">
-        <v>46043.45833333334</v>
+        <v>45994.45833333334</v>
       </c>
       <c r="M200" t="inlineStr">
         <is>
-          <t>£600,000</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N200" s="1" t="n">
-        <v>45931</v>
+        <v>45924</v>
       </c>
     </row>
     <row r="201">
@@ -12192,21 +12254,21 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Feasibility studies 2</t>
+          <t>Eureka GlobalStars Japan 2026</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2307/overview/8eec43e7-96a5-49d1-97e1-3400321160f9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2276/overview/19635c62-dd91-41d8-a90e-547cdb5acbfa</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>2025-10-10 08:18</t>
+          <t>2025-10-03 08:17</t>
         </is>
       </c>
       <c r="E201" s="1" t="n">
-        <v>45940.34583333333</v>
+        <v>45933.34513888889</v>
       </c>
       <c r="F201" t="b">
         <v>1</v>
@@ -12219,19 +12281,19 @@
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 21 January 2026 11:00am</t>
         </is>
       </c>
       <c r="L201" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46043.45833333334</v>
       </c>
       <c r="M201" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£600,000</t>
         </is>
       </c>
       <c r="N201" s="1" t="n">
-        <v>45938</v>
+        <v>45931</v>
       </c>
     </row>
     <row r="202">
@@ -12242,21 +12304,21 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch EoI – October 2025</t>
+          <t>CAM Pathfinder: Feasibility studies 2</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2317/overview/c946fbde-725e-4f85-bb3f-3219576c4a01</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2307/overview/8eec43e7-96a5-49d1-97e1-3400321160f9</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>2025-10-14 08:17</t>
+          <t>2025-10-10 08:18</t>
         </is>
       </c>
       <c r="E202" s="1" t="n">
-        <v>45944.34513888889</v>
+        <v>45940.34583333333</v>
       </c>
       <c r="F202" t="b">
         <v>1</v>
@@ -12269,13 +12331,17 @@
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr">
         <is>
-          <t>Wednesday 22 October 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L202" s="1" t="n">
-        <v>45952.45833333334</v>
-      </c>
-      <c r="M202" t="inlineStr"/>
+        <v>45987.45833333334</v>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>£250,000</t>
+        </is>
+      </c>
       <c r="N202" s="1" t="n">
         <v>45938</v>
       </c>
@@ -12288,21 +12354,21 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Enable</t>
+          <t>ATI Programme strategic batch EoI – October 2025</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2318/overview/39cd0e04-6f9c-40da-b0be-8eaae7f1603d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2317/overview/c946fbde-725e-4f85-bb3f-3219576c4a01</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>2025-10-15 08:19</t>
+          <t>2025-10-14 08:17</t>
         </is>
       </c>
       <c r="E203" s="1" t="n">
-        <v>45945.34652777778</v>
+        <v>45944.34513888889</v>
       </c>
       <c r="F203" t="b">
         <v>1</v>
@@ -12315,19 +12381,15 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 22 October 2025 11:00am</t>
         </is>
       </c>
       <c r="L203" s="1" t="n">
-        <v>46008.45833333334</v>
-      </c>
-      <c r="M203" t="inlineStr">
-        <is>
-          <t>£4.0 million</t>
-        </is>
-      </c>
+        <v>45952.45833333334</v>
+      </c>
+      <c r="M203" t="inlineStr"/>
       <c r="N203" s="1" t="n">
-        <v>45945</v>
+        <v>45938</v>
       </c>
     </row>
     <row r="204">
@@ -12338,12 +12400,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>CAM Pathfinder: Demonstrate</t>
+          <t>CAM Pathfinder: Enable</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2315/overview/f02885bb-e043-4a60-8d0c-22242bd77fa9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2318/overview/39cd0e04-6f9c-40da-b0be-8eaae7f1603d</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -12373,7 +12435,7 @@
       </c>
       <c r="M204" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£4.0 million</t>
         </is>
       </c>
       <c r="N204" s="1" t="n">
@@ -12388,21 +12450,21 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Launchpad: life and health sciences, Northern Ireland – Rd3 MFA</t>
+          <t>CAM Pathfinder: Demonstrate</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2305/overview/fe565f48-36a8-4d8b-8515-e89d750f259c</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2315/overview/f02885bb-e043-4a60-8d0c-22242bd77fa9</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>2025-10-16 08:19</t>
+          <t>2025-10-15 08:19</t>
         </is>
       </c>
       <c r="E205" s="1" t="n">
-        <v>45946.34652777778</v>
+        <v>45945.34652777778</v>
       </c>
       <c r="F205" t="b">
         <v>1</v>
@@ -12415,15 +12477,15 @@
       <c r="J205" t="inlineStr"/>
       <c r="K205" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L205" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M205" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N205" s="1" t="n">
@@ -12438,21 +12500,21 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 5</t>
+          <t>Launchpad: life and health sciences, Northern Ireland – Rd3 MFA</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2299/overview/0a26e49f-fa03-4096-aa8b-3eb39b68f20d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2305/overview/fe565f48-36a8-4d8b-8515-e89d750f259c</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>2025-10-17 08:19</t>
+          <t>2025-10-16 08:19</t>
         </is>
       </c>
       <c r="E206" s="1" t="n">
-        <v>45947.34652777778</v>
+        <v>45946.34652777778</v>
       </c>
       <c r="F206" t="b">
         <v>1</v>
@@ -12473,7 +12535,7 @@
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N206" s="1" t="n">
@@ -12488,21 +12550,21 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Battery Innovation Feasibility Studies Round 1</t>
+          <t>ADOPT Facilitator Support Grant: Round 5</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2313/overview/508ab35f-0e07-4e84-8e31-bbbcb619bc9e</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2299/overview/0a26e49f-fa03-4096-aa8b-3eb39b68f20d</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>2025-10-18 08:16</t>
+          <t>2025-10-17 08:19</t>
         </is>
       </c>
       <c r="E207" s="1" t="n">
-        <v>45948.34444444445</v>
+        <v>45947.34652777778</v>
       </c>
       <c r="F207" t="b">
         <v>1</v>
@@ -12515,15 +12577,15 @@
       <c r="J207" t="inlineStr"/>
       <c r="K207" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L207" s="1" t="n">
-        <v>46008.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M207" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N207" s="1" t="n">
@@ -12538,12 +12600,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Battery Innovation Concept Development Round 1</t>
+          <t>Battery Innovation Feasibility Studies Round 1</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2314/overview/4d1e65d7-b380-41b7-8dcf-b25cd26b9ab5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2313/overview/508ab35f-0e07-4e84-8e31-bbbcb619bc9e</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -12573,7 +12635,7 @@
       </c>
       <c r="M208" t="inlineStr">
         <is>
-          <t>£4.0 million</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N208" s="1" t="n">
@@ -12588,21 +12650,21 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>The Agentic AI Pioneers Prize</t>
+          <t>Battery Innovation Concept Development Round 1</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2316/overview/fa0eeab0-3021-4cbc-8975-5bd45a7d642a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2314/overview/4d1e65d7-b380-41b7-8dcf-b25cd26b9ab5</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>2025-10-21 08:20</t>
+          <t>2025-10-18 08:16</t>
         </is>
       </c>
       <c r="E209" s="1" t="n">
-        <v>45951.34722222222</v>
+        <v>45948.34444444445</v>
       </c>
       <c r="F209" t="b">
         <v>1</v>
@@ -12615,13 +12677,17 @@
       <c r="J209" t="inlineStr"/>
       <c r="K209" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L209" s="1" t="n">
-        <v>45980.45833333334</v>
-      </c>
-      <c r="M209" t="inlineStr"/>
+        <v>46008.45833333334</v>
+      </c>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t>£4.0 million</t>
+        </is>
+      </c>
       <c r="N209" s="1" t="n">
         <v>45945</v>
       </c>
@@ -12634,21 +12700,21 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>MSI: SME resource and energy efficiency – industrial research</t>
+          <t>The Agentic AI Pioneers Prize</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2328/overview/79cb058a-71b3-459a-93c2-8c96ecf7f18a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2316/overview/fa0eeab0-3021-4cbc-8975-5bd45a7d642a</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>2025-10-22 08:21</t>
+          <t>2025-10-21 08:20</t>
         </is>
       </c>
       <c r="E210" s="1" t="n">
-        <v>45952.34791666667</v>
+        <v>45951.34722222222</v>
       </c>
       <c r="F210" t="b">
         <v>1</v>
@@ -12661,19 +12727,15 @@
       <c r="J210" t="inlineStr"/>
       <c r="K210" t="inlineStr">
         <is>
-          <t>Wednesday 10 December 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L210" s="1" t="n">
-        <v>46001.45833333334</v>
-      </c>
-      <c r="M210" t="inlineStr">
-        <is>
-          <t>£1.0 million</t>
-        </is>
-      </c>
+        <v>45980.45833333334</v>
+      </c>
+      <c r="M210" t="inlineStr"/>
       <c r="N210" s="1" t="n">
-        <v>45952</v>
+        <v>45945</v>
       </c>
     </row>
     <row r="211">
@@ -12684,12 +12746,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>MSI: SME resource and energy   efficiency – feasibility studies</t>
+          <t>MSI: SME resource and energy efficiency – industrial research</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2327/overview/bd7d1a37-69dc-4d09-8615-2bae4bcf3666</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2328/overview/79cb058a-71b3-459a-93c2-8c96ecf7f18a</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -12719,7 +12781,7 @@
       </c>
       <c r="M211" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£1.0 million</t>
         </is>
       </c>
       <c r="N211" s="1" t="n">
@@ -12734,21 +12796,21 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant Round 4</t>
+          <t>MSI: SME resource and energy   efficiency – feasibility studies</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2298/overview/71fd7055-502d-4f85-9127-749156a80fe6</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2327/overview/bd7d1a37-69dc-4d09-8615-2bae4bcf3666</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>2025-10-23 08:19</t>
+          <t>2025-10-22 08:21</t>
         </is>
       </c>
       <c r="E212" s="1" t="n">
-        <v>45953.34652777778</v>
+        <v>45952.34791666667</v>
       </c>
       <c r="F212" t="b">
         <v>1</v>
@@ -12769,7 +12831,7 @@
       </c>
       <c r="M212" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N212" s="1" t="n">
@@ -12784,21 +12846,21 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 24</t>
+          <t>Full ADOPT Grant Round 4</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2322/overview/1b933876-5f58-4dec-85ab-68b8c2722211</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2298/overview/71fd7055-502d-4f85-9127-749156a80fe6</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>2025-10-24 08:19</t>
+          <t>2025-10-23 08:19</t>
         </is>
       </c>
       <c r="E213" s="1" t="n">
-        <v>45954.34652777778</v>
+        <v>45953.34652777778</v>
       </c>
       <c r="F213" t="b">
         <v>1</v>
@@ -12811,15 +12873,15 @@
       <c r="J213" t="inlineStr"/>
       <c r="K213" t="inlineStr">
         <is>
-          <t>Wednesday 7 January 2026 11:00am</t>
+          <t>Wednesday 10 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L213" s="1" t="n">
-        <v>46029.45833333334</v>
+        <v>46001.45833333334</v>
       </c>
       <c r="M213" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N213" s="1" t="n">
@@ -12834,21 +12896,21 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 4</t>
+          <t>Innovate UK Innovation Loans Round 24</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2290/overview/8dd45f5c-3f38-4e38-b733-42b6cf601292</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2322/overview/1b933876-5f58-4dec-85ab-68b8c2722211</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>2025-10-25 08:16</t>
+          <t>2025-10-24 08:19</t>
         </is>
       </c>
       <c r="E214" s="1" t="n">
-        <v>45955.34444444445</v>
+        <v>45954.34652777778</v>
       </c>
       <c r="F214" t="b">
         <v>1</v>
@@ -12861,15 +12923,15 @@
       <c r="J214" t="inlineStr"/>
       <c r="K214" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 7 January 2026 11:00am</t>
         </is>
       </c>
       <c r="L214" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46029.45833333334</v>
       </c>
       <c r="M214" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N214" s="1" t="n">
@@ -12884,21 +12946,21 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>National Materials Innovation Programme: Feasibility Studies</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 4</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2326/overview/ca8aab61-a03b-431f-94a8-5c9b008495d5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2290/overview/8dd45f5c-3f38-4e38-b733-42b6cf601292</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>2025-10-31 08:18</t>
+          <t>2025-10-25 08:16</t>
         </is>
       </c>
       <c r="E215" s="1" t="n">
-        <v>45961.34583333333</v>
+        <v>45955.34444444445</v>
       </c>
       <c r="F215" t="b">
         <v>1</v>
@@ -12911,19 +12973,19 @@
       <c r="J215" t="inlineStr"/>
       <c r="K215" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L215" s="1" t="n">
-        <v>46008.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M215" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N215" s="1" t="n">
-        <v>45959</v>
+        <v>45952</v>
       </c>
     </row>
     <row r="216">
@@ -12934,21 +12996,21 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>UK-Canada Quantum Communications and Networking Demonstrator</t>
+          <t>National Materials Innovation Programme: Feasibility Studies</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2335/overview/64e26f1b-8564-4539-b3ca-1b15ebf4f94a</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2326/overview/ca8aab61-a03b-431f-94a8-5c9b008495d5</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>2025-11-04 08:20</t>
+          <t>2025-10-31 08:18</t>
         </is>
       </c>
       <c r="E216" s="1" t="n">
-        <v>45965.34722222222</v>
+        <v>45961.34583333333</v>
       </c>
       <c r="F216" t="b">
         <v>1</v>
@@ -12961,15 +13023,15 @@
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr">
         <is>
-          <t>Wednesday 26 November 2025 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L216" s="1" t="n">
-        <v>45987.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M216" t="inlineStr">
         <is>
-          <t>£3.4 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N216" s="1" t="n">
@@ -12984,12 +13046,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Increasing EV charging capacity on the strategic road network</t>
+          <t>UK-Canada Quantum Communications and Networking Demonstrator</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2304/overview/9ea6670e-83fd-43f9-972f-e0eff8fe77a8</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2335/overview/64e26f1b-8564-4539-b3ca-1b15ebf4f94a</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -13011,15 +13073,15 @@
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Wednesday 26 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L217" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>45987.45833333334</v>
       </c>
       <c r="M217" t="inlineStr">
         <is>
-          <t>£3.0 million</t>
+          <t>£3.4 million</t>
         </is>
       </c>
       <c r="N217" s="1" t="n">
@@ -13034,21 +13096,21 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst 2025: Industry led R&amp;D small projects</t>
+          <t>Increasing EV charging capacity on the strategic road network</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2333/overview/f5431c75-e2e1-48f4-bc8e-62d52121cb6f</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2304/overview/9ea6670e-83fd-43f9-972f-e0eff8fe77a8</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>2025-11-05 08:19</t>
+          <t>2025-11-04 08:20</t>
         </is>
       </c>
       <c r="E218" s="1" t="n">
-        <v>45966.34652777778</v>
+        <v>45965.34722222222</v>
       </c>
       <c r="F218" t="b">
         <v>1</v>
@@ -13061,19 +13123,19 @@
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr">
         <is>
-          <t>Wednesday 10 December 2025 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L218" s="1" t="n">
-        <v>46001.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M218" t="inlineStr">
         <is>
-          <t>£1.0 million</t>
+          <t>£3.0 million</t>
         </is>
       </c>
       <c r="N218" s="1" t="n">
-        <v>45966</v>
+        <v>45959</v>
       </c>
     </row>
     <row r="219">
@@ -13084,12 +13146,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst 2025: Industry led R&amp;D large projects</t>
+          <t>Biomedical Catalyst 2025: Industry led R&amp;D small projects</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2332/overview/bf6bd8c3-e550-478d-b374-a3cb0fb4d3d3</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2333/overview/f5431c75-e2e1-48f4-bc8e-62d52121cb6f</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -13119,7 +13181,7 @@
       </c>
       <c r="M219" t="inlineStr">
         <is>
-          <t>£4.0 million</t>
+          <t>£1.0 million</t>
         </is>
       </c>
       <c r="N219" s="1" t="n">
@@ -13134,12 +13196,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>ATI Programme strategic batch EoI – November 2025</t>
+          <t>Biomedical Catalyst 2025: Industry led R&amp;D large projects</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2334/overview/4af06b80-2953-4cb3-8cc0-987ec5a2f322</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2332/overview/bf6bd8c3-e550-478d-b374-a3cb0fb4d3d3</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -13161,13 +13223,17 @@
       <c r="J220" t="inlineStr"/>
       <c r="K220" t="inlineStr">
         <is>
-          <t>Wednesday 19 November 2025 11:00am</t>
+          <t>Wednesday 10 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L220" s="1" t="n">
-        <v>45980.45833333334</v>
-      </c>
-      <c r="M220" t="inlineStr"/>
+        <v>46001.45833333334</v>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>£4.0 million</t>
+        </is>
+      </c>
       <c r="N220" s="1" t="n">
         <v>45966</v>
       </c>
@@ -13180,21 +13246,21 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>DRIVE35 Scale-up: Feasibility Studies 2</t>
+          <t>ATI Programme strategic batch EoI – November 2025</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2341/overview/4b0efce9-75b8-4e84-97c0-fc6277396586</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2334/overview/4af06b80-2953-4cb3-8cc0-987ec5a2f322</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>2025-11-11 08:19</t>
+          <t>2025-11-05 08:19</t>
         </is>
       </c>
       <c r="E221" s="1" t="n">
-        <v>45972.34652777778</v>
+        <v>45966.34652777778</v>
       </c>
       <c r="F221" t="b">
         <v>1</v>
@@ -13207,17 +13273,13 @@
       <c r="J221" t="inlineStr"/>
       <c r="K221" t="inlineStr">
         <is>
-          <t>Wednesday 17 December 2025 11:00am</t>
+          <t>Wednesday 19 November 2025 11:00am</t>
         </is>
       </c>
       <c r="L221" s="1" t="n">
-        <v>46008.45833333334</v>
-      </c>
-      <c r="M221" t="inlineStr">
-        <is>
-          <t>£750,000</t>
-        </is>
-      </c>
+        <v>45980.45833333334</v>
+      </c>
+      <c r="M221" t="inlineStr"/>
       <c r="N221" s="1" t="n">
         <v>45966</v>
       </c>
@@ -13230,21 +13292,21 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Women in Innovation Awards 2025/26</t>
+          <t>DRIVE35 Scale-up: Feasibility Studies 2</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2337/overview/3750b1cd-2080-4a1c-82c0-003fbaafdd2d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2341/overview/4b0efce9-75b8-4e84-97c0-fc6277396586</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>2025-11-27 13:23</t>
+          <t>2025-11-11 08:19</t>
         </is>
       </c>
       <c r="E222" s="1" t="n">
-        <v>45988.55763888889</v>
+        <v>45972.34652777778</v>
       </c>
       <c r="F222" t="b">
         <v>1</v>
@@ -13257,19 +13319,19 @@
       <c r="J222" t="inlineStr"/>
       <c r="K222" t="inlineStr">
         <is>
-          <t>Wednesday 4 February 2026 11:00am</t>
+          <t>Wednesday 17 December 2025 11:00am</t>
         </is>
       </c>
       <c r="L222" s="1" t="n">
-        <v>46057.45833333334</v>
+        <v>46008.45833333334</v>
       </c>
       <c r="M222" t="inlineStr">
         <is>
-          <t>£75,000</t>
+          <t>£750,000</t>
         </is>
       </c>
       <c r="N222" s="1" t="n">
-        <v>45987</v>
+        <v>45966</v>
       </c>
     </row>
     <row r="223">
@@ -13280,21 +13342,21 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 5</t>
+          <t>Women in Innovation Awards 2025/26</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2354/overview/c7008321-f651-45c5-a409-c3215231fbb4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2337/overview/3750b1cd-2080-4a1c-82c0-003fbaafdd2d</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>2025-12-02 08:22</t>
+          <t>2025-11-27 13:23</t>
         </is>
       </c>
       <c r="E223" s="1" t="n">
-        <v>45993.34861111111</v>
+        <v>45988.55763888889</v>
       </c>
       <c r="F223" t="b">
         <v>1</v>
@@ -13315,7 +13377,7 @@
       </c>
       <c r="M223" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£75,000</t>
         </is>
       </c>
       <c r="N223" s="1" t="n">
@@ -13330,21 +13392,21 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Innovate UK Growth Catalyst – Investor Partnerships Round 2</t>
+          <t>Knowledge Transfer Partnership (KTP): 2025 – 2026 Round 5</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2360/overview/37d8f6e1-5600-4e9e-bbfc-11bc320f8808</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2354/overview/c7008321-f651-45c5-a409-c3215231fbb4</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>2025-12-11 08:22</t>
+          <t>2025-12-02 08:22</t>
         </is>
       </c>
       <c r="E224" s="1" t="n">
-        <v>46002.34861111111</v>
+        <v>45993.34861111111</v>
       </c>
       <c r="F224" t="b">
         <v>1</v>
@@ -13357,19 +13419,19 @@
       <c r="J224" t="inlineStr"/>
       <c r="K224" t="inlineStr">
         <is>
-          <t>Tuesday 3 February 2026 11:00am</t>
+          <t>Wednesday 4 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L224" s="1" t="n">
-        <v>46056.45833333334</v>
+        <v>46057.45833333334</v>
       </c>
       <c r="M224" t="inlineStr">
         <is>
-          <t>£2.0 million</t>
+          <t>£8,500</t>
         </is>
       </c>
       <c r="N224" s="1" t="n">
-        <v>46001</v>
+        <v>45987</v>
       </c>
     </row>
     <row r="225">
@@ -13380,21 +13442,21 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 5</t>
+          <t>Innovate UK Growth Catalyst – Investor Partnerships Round 2</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2358/overview/f93f32c2-dd04-474d-bc35-a8af1ecac1a9</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2360/overview/37d8f6e1-5600-4e9e-bbfc-11bc320f8808</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>2025-12-12 08:22</t>
+          <t>2025-12-11 08:22</t>
         </is>
       </c>
       <c r="E225" s="1" t="n">
-        <v>46003.34861111111</v>
+        <v>46002.34861111111</v>
       </c>
       <c r="F225" t="b">
         <v>1</v>
@@ -13407,15 +13469,15 @@
       <c r="J225" t="inlineStr"/>
       <c r="K225" t="inlineStr">
         <is>
-          <t>Wednesday 4 February 2026 11:00am</t>
+          <t>Tuesday 3 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L225" s="1" t="n">
-        <v>46057.45833333334</v>
+        <v>46056.45833333334</v>
       </c>
       <c r="M225" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£2.0 million</t>
         </is>
       </c>
       <c r="N225" s="1" t="n">
@@ -13430,21 +13492,21 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>ADOPT Facilitator Support Grant: Round 6</t>
+          <t>Full ADOPT Grant: Round 5</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2371/overview/471bfe91-9f9c-4086-a28a-15296f1957e2</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2358/overview/f93f32c2-dd04-474d-bc35-a8af1ecac1a9</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>2025-12-18 08:21</t>
+          <t>2025-12-12 08:22</t>
         </is>
       </c>
       <c r="E226" s="1" t="n">
-        <v>46009.34791666667</v>
+        <v>46003.34861111111</v>
       </c>
       <c r="F226" t="b">
         <v>1</v>
@@ -13457,19 +13519,19 @@
       <c r="J226" t="inlineStr"/>
       <c r="K226" t="inlineStr">
         <is>
-          <t>Wednesday 25 February 2026 11:00am</t>
+          <t>Wednesday 4 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L226" s="1" t="n">
-        <v>46078.45833333334</v>
+        <v>46057.45833333334</v>
       </c>
       <c r="M226" t="inlineStr">
         <is>
-          <t>£2,500</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N226" s="1" t="n">
-        <v>46008</v>
+        <v>46001</v>
       </c>
     </row>
     <row r="227">
@@ -13480,12 +13542,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Commercialising Knowledge Assets Fund (CKAF) Spring</t>
+          <t>ADOPT Facilitator Support Grant: Round 6</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2369/overview/abf7d399-81b9-4f33-b592-51825a288c37</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2371/overview/471bfe91-9f9c-4086-a28a-15296f1957e2</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -13507,15 +13569,15 @@
       <c r="J227" t="inlineStr"/>
       <c r="K227" t="inlineStr">
         <is>
-          <t>Thursday 7 May 2026 11:00am</t>
+          <t>Wednesday 25 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L227" s="1" t="n">
-        <v>46149.45833333334</v>
+        <v>46078.45833333334</v>
       </c>
       <c r="M227" t="inlineStr">
         <is>
-          <t>£250,000</t>
+          <t>£2,500</t>
         </is>
       </c>
       <c r="N227" s="1" t="n">
@@ -13530,21 +13592,21 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – mid stage</t>
+          <t>Commercialising Knowledge Assets Fund (CKAF) Spring</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2363/overview/9f759af1-3732-4d15-995d-053e28025d22</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2369/overview/abf7d399-81b9-4f33-b592-51825a288c37</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>2026-01-06 08:22</t>
+          <t>2025-12-18 08:21</t>
         </is>
       </c>
       <c r="E228" s="1" t="n">
-        <v>46028.34861111111</v>
+        <v>46009.34791666667</v>
       </c>
       <c r="F228" t="b">
         <v>1</v>
@@ -13557,19 +13619,19 @@
       <c r="J228" t="inlineStr"/>
       <c r="K228" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Thursday 7 May 2026 11:00am</t>
         </is>
       </c>
       <c r="L228" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>46149.45833333334</v>
       </c>
       <c r="M228" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£250,000</t>
         </is>
       </c>
       <c r="N228" s="1" t="n">
-        <v>46022</v>
+        <v>46008</v>
       </c>
     </row>
     <row r="229">
@@ -13580,12 +13642,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – late stage</t>
+          <t>Energy catalyst round 11 – mid stage</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2364/overview/b9d4dedf-d22a-41d1-9ca2-6c5a279519be</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2363/overview/9f759af1-3732-4d15-995d-053e28025d22</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -13615,7 +13677,7 @@
       </c>
       <c r="M229" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N229" s="1" t="n">
@@ -13630,12 +13692,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Energy catalyst round 11 – early stage</t>
+          <t>Energy catalyst round 11 – late stage</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2362/overview/640b2f4e-8571-4aef-9e2a-67e35db3db77</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2364/overview/b9d4dedf-d22a-41d1-9ca2-6c5a279519be</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -13665,7 +13727,7 @@
       </c>
       <c r="M230" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N230" s="1" t="n">
@@ -13680,12 +13742,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Demonstrate 2</t>
+          <t>Energy catalyst round 11 – early stage</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2351/overview/349c38f5-5ed2-4cf4-a324-bda2d6cd1e67</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2362/overview/640b2f4e-8571-4aef-9e2a-67e35db3db77</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -13707,15 +13769,15 @@
       <c r="J231" t="inlineStr"/>
       <c r="K231" t="inlineStr">
         <is>
-          <t>Wednesday 11 March 2026 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L231" s="1" t="n">
-        <v>46092.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M231" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N231" s="1" t="n">
@@ -13730,12 +13792,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>DRIVE35 Innovation Fund: Collaborate 2</t>
+          <t>DRIVE35 Innovation Fund: Demonstrate 2</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2350/overview/dbd41be3-14ea-4c83-8774-eb28a8703d57</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2351/overview/349c38f5-5ed2-4cf4-a324-bda2d6cd1e67</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -13757,15 +13819,15 @@
       <c r="J232" t="inlineStr"/>
       <c r="K232" t="inlineStr">
         <is>
-          <t>Wednesday 18 March 2026 11:00am</t>
+          <t>Wednesday 11 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L232" s="1" t="n">
-        <v>46099.45833333334</v>
+        <v>46092.45833333334</v>
       </c>
       <c r="M232" t="inlineStr">
         <is>
-          <t>£25.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N232" s="1" t="n">
@@ -13780,21 +13842,21 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Innovate UK Innovation Loans Round 25</t>
+          <t>DRIVE35 Innovation Fund: Collaborate 2</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2373/overview/609dc5dd-d3e8-4f51-af3a-3eb1b3314710</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2350/overview/dbd41be3-14ea-4c83-8774-eb28a8703d57</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>2026-01-08 08:22</t>
+          <t>2026-01-06 08:22</t>
         </is>
       </c>
       <c r="E233" s="1" t="n">
-        <v>46030.34861111111</v>
+        <v>46028.34861111111</v>
       </c>
       <c r="F233" t="b">
         <v>1</v>
@@ -13807,19 +13869,19 @@
       <c r="J233" t="inlineStr"/>
       <c r="K233" t="inlineStr">
         <is>
-          <t>Wednesday 4 March 2026 11:00am</t>
+          <t>Wednesday 18 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L233" s="1" t="n">
-        <v>46085.45833333334</v>
+        <v>46099.45833333334</v>
       </c>
       <c r="M233" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£25.0 million</t>
         </is>
       </c>
       <c r="N233" s="1" t="n">
-        <v>46029</v>
+        <v>46022</v>
       </c>
     </row>
     <row r="234">
@@ -13830,21 +13892,21 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Cyber Security Academic Startup Accelerator Programme Y10 Phase 1</t>
+          <t>Innovate UK Innovation Loans Round 25</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2376/overview/1b9b9265-ca4b-4f8c-a0c2-577cb8713642</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2373/overview/609dc5dd-d3e8-4f51-af3a-3eb1b3314710</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>2026-01-15 08:23</t>
+          <t>2026-01-08 08:22</t>
         </is>
       </c>
       <c r="E234" s="1" t="n">
-        <v>46037.34930555556</v>
+        <v>46030.34861111111</v>
       </c>
       <c r="F234" t="b">
         <v>1</v>
@@ -13857,19 +13919,19 @@
       <c r="J234" t="inlineStr"/>
       <c r="K234" t="inlineStr">
         <is>
-          <t>Wednesday 11 February 2026 11:00am</t>
+          <t>Wednesday 4 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L234" s="1" t="n">
-        <v>46064.45833333334</v>
+        <v>46085.45833333334</v>
       </c>
       <c r="M234" t="inlineStr">
         <is>
-          <t>£32,000</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N234" s="1" t="n">
-        <v>46036</v>
+        <v>46029</v>
       </c>
     </row>
     <row r="235">
@@ -13880,21 +13942,21 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C5</t>
+          <t>Cyber Security Academic Startup Accelerator Programme Y10 Phase 1</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2346/overview/e172ee7c-3050-4d47-bf11-235cfe76c1e1</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2376/overview/1b9b9265-ca4b-4f8c-a0c2-577cb8713642</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>2026-01-20 08:24</t>
+          <t>2026-01-15 08:23</t>
         </is>
       </c>
       <c r="E235" s="1" t="n">
-        <v>46042.35</v>
+        <v>46037.34930555556</v>
       </c>
       <c r="F235" t="b">
         <v>1</v>
@@ -13907,15 +13969,15 @@
       <c r="J235" t="inlineStr"/>
       <c r="K235" t="inlineStr">
         <is>
-          <t>Wednesday 25 February 2026 11:00am</t>
+          <t>Wednesday 11 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L235" s="1" t="n">
-        <v>46078.45833333334</v>
+        <v>46064.45833333334</v>
       </c>
       <c r="M235" t="inlineStr">
         <is>
-          <t>£150,000</t>
+          <t>£32,000</t>
         </is>
       </c>
       <c r="N235" s="1" t="n">
@@ -13930,21 +13992,21 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Advanced manufacturing supply chain innovation FS</t>
+          <t>Ofgem Strategic Innovation Fund Round 5 Discovery C5</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2384/overview/2ad8ce21-d3f6-48bf-b55a-5af2a892a1e0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2346/overview/e172ee7c-3050-4d47-bf11-235cfe76c1e1</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>2026-01-26 12:10</t>
+          <t>2026-01-20 08:24</t>
         </is>
       </c>
       <c r="E236" s="1" t="n">
-        <v>46048.50694444445</v>
+        <v>46042.35</v>
       </c>
       <c r="F236" t="b">
         <v>1</v>
@@ -13957,19 +14019,19 @@
       <c r="J236" t="inlineStr"/>
       <c r="K236" t="inlineStr">
         <is>
-          <t>Wednesday 11 March 2026 11:00am</t>
+          <t>Wednesday 25 February 2026 11:00am</t>
         </is>
       </c>
       <c r="L236" s="1" t="n">
-        <v>46092.45833333334</v>
+        <v>46078.45833333334</v>
       </c>
       <c r="M236" t="inlineStr">
         <is>
-          <t>£100,000</t>
+          <t>£150,000</t>
         </is>
       </c>
       <c r="N236" s="1" t="n">
-        <v>46043</v>
+        <v>46036</v>
       </c>
     </row>
     <row r="237">
@@ -13980,21 +14042,21 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>TechLocal: Connecting Local Talent to Local Tech Jobs</t>
+          <t>Advanced manufacturing supply chain innovation FS</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2378/overview/ae120ce2-7b72-4cf2-8dde-f78b02d5996d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2384/overview/2ad8ce21-d3f6-48bf-b55a-5af2a892a1e0</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>2026-01-28 10:24</t>
+          <t>2026-01-26 12:10</t>
         </is>
       </c>
       <c r="E237" s="1" t="n">
-        <v>46050.43333333333</v>
+        <v>46048.50694444445</v>
       </c>
       <c r="F237" t="b">
         <v>1</v>
@@ -14007,19 +14069,19 @@
       <c r="J237" t="inlineStr"/>
       <c r="K237" t="inlineStr">
         <is>
-          <t>Wednesday 18 March 2026 11:00am</t>
+          <t>Wednesday 11 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L237" s="1" t="n">
-        <v>46099.45833333334</v>
+        <v>46092.45833333334</v>
       </c>
       <c r="M237" t="inlineStr">
         <is>
-          <t>£225,000</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N237" s="1" t="n">
-        <v>46050</v>
+        <v>46043</v>
       </c>
     </row>
     <row r="238">
@@ -14030,12 +14092,12 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>TechLocal AI Professional Degree and Traineeship Accelerator</t>
+          <t>TechLocal: Connecting Local Talent to Local Tech Jobs</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2375/overview/6431359e-eb5c-4f76-b49d-299948107fbd</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2378/overview/ae120ce2-7b72-4cf2-8dde-f78b02d5996d</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -14065,7 +14127,7 @@
       </c>
       <c r="M238" t="inlineStr">
         <is>
-          <t>£300,000</t>
+          <t>£225,000</t>
         </is>
       </c>
       <c r="N238" s="1" t="n">
@@ -14080,21 +14142,21 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Robotics Adoption Programme skills development</t>
+          <t>TechLocal AI Professional Degree and Traineeship Accelerator</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2387/overview/daca31c2-8395-4bc2-a5da-55eb1e432fa4</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2375/overview/6431359e-eb5c-4f76-b49d-299948107fbd</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>2026-02-02 10:39</t>
+          <t>2026-01-28 10:24</t>
         </is>
       </c>
       <c r="E239" s="1" t="n">
-        <v>46055.44375</v>
+        <v>46050.43333333333</v>
       </c>
       <c r="F239" t="b">
         <v>1</v>
@@ -14107,15 +14169,15 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr">
         <is>
-          <t>Wednesday 25 March 2026 11:00am</t>
+          <t>Wednesday 18 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L239" s="1" t="n">
-        <v>46106.45833333334</v>
+        <v>46099.45833333334</v>
       </c>
       <c r="M239" t="inlineStr">
         <is>
-          <t>£500,000</t>
+          <t>£300,000</t>
         </is>
       </c>
       <c r="N239" s="1" t="n">
@@ -14130,21 +14192,21 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Knowledge Transfer Partnership (KTP): 2026 – 2027 Round 1</t>
+          <t>Robotics Adoption Programme skills development</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2380/overview/3e170dd3-4458-4c7e-a096-e0ea50b88040</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2387/overview/daca31c2-8395-4bc2-a5da-55eb1e432fa4</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>2026-02-03 10:35</t>
+          <t>2026-02-02 10:39</t>
         </is>
       </c>
       <c r="E240" s="1" t="n">
-        <v>46056.44097222222</v>
+        <v>46055.44375</v>
       </c>
       <c r="F240" t="b">
         <v>1</v>
@@ -14157,15 +14219,15 @@
       <c r="J240" t="inlineStr"/>
       <c r="K240" t="inlineStr">
         <is>
-          <t>Wednesday 1 April 2026 11:00am</t>
+          <t>Wednesday 25 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L240" s="1" t="n">
-        <v>46113.45833333334</v>
+        <v>46106.45833333334</v>
       </c>
       <c r="M240" t="inlineStr">
         <is>
-          <t>£8,500</t>
+          <t>£500,000</t>
         </is>
       </c>
       <c r="N240" s="1" t="n">
@@ -14180,12 +14242,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst Accelerator Provider Pool EoI: late stage</t>
+          <t>Knowledge Transfer Partnership (KTP): 2026 – 2027 Round 1</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2389/overview/a7f7d874-8b6b-45d6-b1e1-1e88e11a1ea5</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2380/overview/3e170dd3-4458-4c7e-a096-e0ea50b88040</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -14207,13 +14269,17 @@
       <c r="J241" t="inlineStr"/>
       <c r="K241" t="inlineStr">
         <is>
-          <t>Wednesday 4 March 2026 11:00am</t>
+          <t>Wednesday 1 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L241" s="1" t="n">
-        <v>46085.45833333334</v>
-      </c>
-      <c r="M241" t="inlineStr"/>
+        <v>46113.45833333334</v>
+      </c>
+      <c r="M241" t="inlineStr">
+        <is>
+          <t>£8,500</t>
+        </is>
+      </c>
       <c r="N241" s="1" t="n">
         <v>46050</v>
       </c>
@@ -14226,12 +14292,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Biomedical Catalyst Accelerator Provider Pool EoI: early stage</t>
+          <t>Biomedical Catalyst Accelerator Provider Pool EoI: late stage</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2388/overview/08b8ab63-085d-4d79-ae83-e8c1698cb327</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2389/overview/a7f7d874-8b6b-45d6-b1e1-1e88e11a1ea5</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -14272,21 +14338,21 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Full ADOPT Grant: Round 6</t>
+          <t>Biomedical Catalyst Accelerator Provider Pool EoI: early stage</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2385/overview/2343c344-807d-41a1-9551-05ac5420ba11</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2388/overview/08b8ab63-085d-4d79-ae83-e8c1698cb327</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>2026-02-09 10:53</t>
+          <t>2026-02-03 10:35</t>
         </is>
       </c>
       <c r="E243" s="1" t="n">
-        <v>46062.45347222222</v>
+        <v>46056.44097222222</v>
       </c>
       <c r="F243" t="b">
         <v>1</v>
@@ -14299,19 +14365,15 @@
       <c r="J243" t="inlineStr"/>
       <c r="K243" t="inlineStr">
         <is>
-          <t>Wednesday 8 April 2026 11:00am</t>
+          <t>Wednesday 4 March 2026 11:00am</t>
         </is>
       </c>
       <c r="L243" s="1" t="n">
-        <v>46120.45833333334</v>
-      </c>
-      <c r="M243" t="inlineStr">
-        <is>
-          <t>£100,000</t>
-        </is>
-      </c>
+        <v>46085.45833333334</v>
+      </c>
+      <c r="M243" t="inlineStr"/>
       <c r="N243" s="1" t="n">
-        <v>46057</v>
+        <v>46050</v>
       </c>
     </row>
     <row r="244">
@@ -14322,21 +14384,21 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Zero Emission Flight Demonstrator Round 1</t>
+          <t>Full ADOPT Grant: Round 6</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2385/overview/2343c344-807d-41a1-9551-05ac5420ba11</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>2026-02-12 10:40</t>
+          <t>2026-02-09 10:53</t>
         </is>
       </c>
       <c r="E244" s="1" t="n">
-        <v>46065.44444444445</v>
+        <v>46062.45347222222</v>
       </c>
       <c r="F244" t="b">
         <v>1</v>
@@ -14349,19 +14411,19 @@
       <c r="J244" t="inlineStr"/>
       <c r="K244" t="inlineStr">
         <is>
-          <t>Wednesday 1 April 2026 11:00am</t>
+          <t>Wednesday 8 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L244" s="1" t="n">
-        <v>46113.45833333334</v>
+        <v>46120.45833333334</v>
       </c>
       <c r="M244" t="inlineStr">
         <is>
-          <t>£5.0 million</t>
+          <t>£100,000</t>
         </is>
       </c>
       <c r="N244" s="1" t="n">
-        <v>46064</v>
+        <v>46057</v>
       </c>
     </row>
     <row r="245">
@@ -14372,12 +14434,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
+          <t>Zero Emission Flight Demonstrator Round 1</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2397/overview/752074ec-5f01-46d8-863f-596300a11651</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -14399,15 +14461,15 @@
       <c r="J245" t="inlineStr"/>
       <c r="K245" t="inlineStr">
         <is>
-          <t>Wednesday 6 May 2026 11:00am</t>
+          <t>Wednesday 1 April 2026 11:00am</t>
         </is>
       </c>
       <c r="L245" s="1" t="n">
-        <v>46148.45833333334</v>
+        <v>46113.45833333334</v>
       </c>
       <c r="M245" t="inlineStr">
         <is>
-          <t>£1.5 million</t>
+          <t>£5.0 million</t>
         </is>
       </c>
       <c r="N245" s="1" t="n">
@@ -14422,12 +14484,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
+          <t>Contracts for Innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2395/overview/3d49fbc4-6e09-4dd8-9ac8-8e5f88facd8d</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -14457,7 +14519,7 @@
       </c>
       <c r="M246" t="inlineStr">
         <is>
-          <t>£10.0 million</t>
+          <t>£1.5 million</t>
         </is>
       </c>
       <c r="N246" s="1" t="n">
@@ -14472,21 +14534,21 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
+          <t>Advancing innovation in drug and alcohol addiction healthcare</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2394/overview/33b56af8-353f-46ac-bb66-a0928731c0fc</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>2026-02-13 10:35</t>
+          <t>2026-02-12 10:40</t>
         </is>
       </c>
       <c r="E247" s="1" t="n">
-        <v>46066.44097222222</v>
+        <v>46065.44444444445</v>
       </c>
       <c r="F247" t="b">
         <v>1</v>
@@ -14499,18 +14561,68 @@
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr">
         <is>
+          <t>Wednesday 6 May 2026 11:00am</t>
+        </is>
+      </c>
+      <c r="L247" s="1" t="n">
+        <v>46148.45833333334</v>
+      </c>
+      <c r="M247" t="inlineStr">
+        <is>
+          <t>£10.0 million</t>
+        </is>
+      </c>
+      <c r="N247" s="1" t="n">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Innovate Funding Service</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>UK-Germany Collaborative Innovation for Quantum Technologies 2026</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>https://apply-for-innovation-funding.service.gov.uk/competition/2392/overview/b8b93732-6326-4aed-9af3-334e4cc5ecc0</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2026-02-13 10:35</t>
+        </is>
+      </c>
+      <c r="E248" s="1" t="n">
+        <v>46066.44097222222</v>
+      </c>
+      <c r="F248" t="b">
+        <v>1</v>
+      </c>
+      <c r="G248" t="inlineStr"/>
+      <c r="H248" t="b">
+        <v>0</v>
+      </c>
+      <c r="I248" t="inlineStr"/>
+      <c r="J248" t="inlineStr"/>
+      <c r="K248" t="inlineStr">
+        <is>
           <t>Wednesday 15 April 2026 11:00am</t>
         </is>
       </c>
-      <c r="L247" s="1" t="n">
+      <c r="L248" s="1" t="n">
         <v>46127.45833333334</v>
       </c>
-      <c r="M247" t="inlineStr">
+      <c r="M248" t="inlineStr">
         <is>
           <t>£1.0 million</t>
         </is>
       </c>
-      <c r="N247" s="1" t="n">
+      <c r="N248" s="1" t="n">
         <v>46064</v>
       </c>
     </row>
@@ -14557,10 +14669,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
@@ -14583,10 +14695,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C4" t="n">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5">

</xml_diff>